<commit_message>
Actualización User Task Matrix
Se agregaron correcciones en la información.
</commit_message>
<xml_diff>
--- a/User Task/User Task Matrix.xlsx
+++ b/User Task/User Task Matrix.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\Repositorios GitHub\Proyecto Partidon\partidon-documentos-generales\User Task\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="20730" windowHeight="10305"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Matrix" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
   <si>
     <t>User Task</t>
   </si>
@@ -27,45 +30,15 @@
     <t>Importancia</t>
   </si>
   <si>
-    <t>Buscar Establecimientos Deportivos.</t>
-  </si>
-  <si>
-    <t>Crear Campeonatos deportivos.</t>
-  </si>
-  <si>
     <t>Contactar con un establecimiento deportivo para reservar una cancha.</t>
   </si>
   <si>
-    <t>Registrar informacion del establecimiento deportivo.</t>
-  </si>
-  <si>
-    <t>Poder registrar Promociones del establecimiento deportivo.</t>
-  </si>
-  <si>
-    <t>Buscar Campeonatos para participar.</t>
-  </si>
-  <si>
-    <t>Crear Partidos deportivos para jugar con otros deportistas interesados o entre equipos ya conformados .</t>
-  </si>
-  <si>
     <t>Buscar partidos deportivos de mi interes.</t>
   </si>
   <si>
-    <t>Poder juntar a nuestros compañeros de deporte.</t>
-  </si>
-  <si>
-    <t>Poder crear un equipo para jugar en un partido.</t>
-  </si>
-  <si>
-    <t>Poder comunicar noticias con mi equipo sobre nuestro deporte en comun.</t>
-  </si>
-  <si>
     <t>Varias</t>
   </si>
   <si>
-    <t>Algunas</t>
-  </si>
-  <si>
     <t>Nunca</t>
   </si>
   <si>
@@ -87,16 +60,37 @@
     <t>Poco</t>
   </si>
   <si>
-    <t>Perfil Usuario 1 - Fanatico Deportista</t>
-  </si>
-  <si>
-    <t>Perfil Usuario 2 - Dueño del Establecimiento Deportivo</t>
+    <t>Buscar establecimientos deportivos.</t>
+  </si>
+  <si>
+    <t>Registrar información del establecimiento deportivo.</t>
+  </si>
+  <si>
+    <t>Crear un equipo para jugar un partido.</t>
+  </si>
+  <si>
+    <t>Crear partidos para jugar con otros deportistas o entre equipos ya conformados .</t>
+  </si>
+  <si>
+    <t>Juntar a compañeros de deporte.</t>
+  </si>
+  <si>
+    <t>Comunicar noticias con mi equipo.</t>
+  </si>
+  <si>
+    <t>Registrar promociones del establecimiento deportivo.</t>
+  </si>
+  <si>
+    <t>Perfil Usuario 1 - Fanático Deportista</t>
+  </si>
+  <si>
+    <t>Perfil Usuario 2 - Propietario de cancha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,14 +191,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -224,6 +218,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -272,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,18 +513,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H17"/>
+  <dimension ref="B5:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,15 +533,15 @@
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -570,256 +567,210 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>17</v>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -832,28 +783,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>